<commit_message>
unbalanced all feature selection method finished
</commit_message>
<xml_diff>
--- a/Result_sheet_pcos.xlsx
+++ b/Result_sheet_pcos.xlsx
@@ -458,7 +458,7 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M19"/>
+  <dimension ref="A1:M23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2347,105 +2347,416 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>boruta selection</t>
+          <t>Recursive feature selection</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
           <t xml:space="preserve">              precision    recall  f1-score   support
-           0       0.86      0.90      0.88       100
-           1       0.82      0.76      0.79        62
+           0       0.84      0.87      0.85       101
+           1       0.77      0.72      0.75        61
+    accuracy                           0.81       162
+   macro avg       0.81      0.80      0.80       162
+weighted avg       0.81      0.81      0.81       162
+</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t xml:space="preserve">              precision    recall  f1-score   support
+           0       0.87      0.83      0.85       109
+           1       0.68      0.74      0.71        53
+    accuracy                           0.80       162
+   macro avg       0.78      0.79      0.78       162
+weighted avg       0.81      0.80      0.80       162
+</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t xml:space="preserve">              precision    recall  f1-score   support
+           0       0.86      0.83      0.84       109
+           1       0.67      0.72      0.69        53
+    accuracy                           0.79       162
+   macro avg       0.76      0.77      0.77       162
+weighted avg       0.79      0.79      0.79       162
+</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t xml:space="preserve">              precision    recall  f1-score   support
+         0.0       0.91      0.86      0.88       112
+         1.0       0.72      0.82      0.77        50
     accuracy                           0.85       162
-   macro avg       0.84      0.83      0.83       162
-weighted avg       0.84      0.85      0.84       162
-</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t xml:space="preserve">              precision    recall  f1-score   support
-           0       0.91      0.91      0.91       106
-           1       0.82      0.84      0.83        56
-    accuracy                           0.88       162
-   macro avg       0.87      0.87      0.87       162
-weighted avg       0.88      0.88      0.88       162
-</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t xml:space="preserve">              precision    recall  f1-score   support
-         0.0       0.93      0.86      0.89       114
-         1.0       0.72      0.85      0.78        48
-    accuracy                           0.86       162
-   macro avg       0.83      0.86      0.84       162
-weighted avg       0.87      0.86      0.86       162
+   macro avg       0.82      0.84      0.83       162
+weighted avg       0.85      0.85      0.85       162
 </t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
           <t xml:space="preserve">              precision    recall  f1-score   support
-           0       0.94      0.90      0.92       110
-           1       0.81      0.88      0.84        52
-    accuracy                           0.90       162
-   macro avg       0.87      0.89      0.88       162
-weighted avg       0.90      0.90      0.90       162
-</t>
-        </is>
-      </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t xml:space="preserve">              precision    recall  f1-score   support
-           0       0.91      0.87      0.89       110
-           1       0.75      0.83      0.79        52
-    accuracy                           0.86       162
-   macro avg       0.83      0.85      0.84       162
-weighted avg       0.86      0.86      0.86       162
-</t>
-        </is>
-      </c>
-      <c r="H19" t="inlineStr">
-        <is>
-          <t xml:space="preserve">              precision    recall  f1-score   support
-           0       0.95      0.85      0.90       117
-           1       0.70      0.89      0.78        45
-    accuracy                           0.86       162
-   macro avg       0.83      0.87      0.84       162
-weighted avg       0.88      0.86      0.87       162
-</t>
-        </is>
-      </c>
-      <c r="I19" t="inlineStr">
-        <is>
-          <t xml:space="preserve">              precision    recall  f1-score   support
-           0       0.93      0.87      0.90       113
-           1       0.74      0.86      0.79        49
+           0       0.92      0.87      0.90       111
+           1       0.75      0.84      0.80        51
     accuracy                           0.86       162
    macro avg       0.84      0.86      0.85       162
 weighted avg       0.87      0.86      0.87       162
 </t>
         </is>
       </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t xml:space="preserve">              precision    recall  f1-score   support
+           0       0.93      0.83      0.88       118
+           1       0.65      0.84      0.73        44
+    accuracy                           0.83       162
+   macro avg       0.79      0.84      0.81       162
+weighted avg       0.86      0.83      0.84       162
+</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t xml:space="preserve">              precision    recall  f1-score   support
+           0       0.95      0.82      0.88       122
+           1       0.61      0.88      0.72        40
+    accuracy                           0.83       162
+   macro avg       0.78      0.85      0.80       162
+weighted avg       0.87      0.83      0.84       162
+</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t xml:space="preserve">              precision    recall  f1-score   support
+           0       0.90      0.87      0.89       109
+           1       0.75      0.81      0.78        53
+    accuracy                           0.85       162
+   macro avg       0.83      0.84      0.83       162
+weighted avg       0.86      0.85      0.85       162
+</t>
+        </is>
+      </c>
       <c r="J19" t="inlineStr">
         <is>
           <t xml:space="preserve">              precision    recall  f1-score   support
-           0       0.96      0.88      0.92       115
-           1       0.75      0.91      0.83        47
+           0       0.93      0.88      0.90       112
+           1       0.75      0.86      0.80        50
+    accuracy                           0.87       162
+   macro avg       0.84      0.87      0.85       162
+weighted avg       0.88      0.87      0.87       162
+</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t xml:space="preserve">              precision    recall  f1-score   support
+           0       0.94      0.88      0.91       112
+           1       0.77      0.88      0.82        50
+    accuracy                           0.88       162
+   macro avg       0.86      0.88      0.87       162
+weighted avg       0.89      0.88      0.88       162
+</t>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t xml:space="preserve">              precision    recall  f1-score   support
+           0       0.91      0.83      0.87       116
+           1       0.65      0.80      0.72        46
+    accuracy                           0.82       162
+   macro avg       0.78      0.82      0.79       162
+weighted avg       0.84      0.82      0.83       162
+</t>
+        </is>
+      </c>
+      <c r="M19" t="inlineStr">
+        <is>
+          <t xml:space="preserve">              precision    recall  f1-score   support
+           0       0.88      0.88      0.88       105
+           1       0.77      0.77      0.77        57
+    accuracy                           0.84       162
+   macro avg       0.82      0.82      0.82       162
+weighted avg       0.84      0.84      0.84       162
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Chi_Square feature selection</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t xml:space="preserve">              precision    recall  f1-score   support
+           0       0.68      0.89      0.77        80
+           1       0.84      0.59      0.69        82
+    accuracy                           0.73       162
+   macro avg       0.76      0.74      0.73       162
+weighted avg       0.76      0.73      0.73       162
+</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t xml:space="preserve">              precision    recall  f1-score   support
+           0       0.83      0.89      0.86        98
+           1       0.81      0.72      0.76        64
+    accuracy                           0.82       162
+   macro avg       0.82      0.80      0.81       162
+weighted avg       0.82      0.82      0.82       162
+</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t xml:space="preserve">              precision    recall  f1-score   support
+           0       0.72      0.70      0.71       109
+           1       0.42      0.45      0.44        53
+    accuracy                           0.62       162
+   macro avg       0.57      0.58      0.57       162
+weighted avg       0.62      0.62      0.62       162
+</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t xml:space="preserve">              precision    recall  f1-score   support
+         0.0       0.89      0.94      0.91        99
+         1.0       0.89      0.81      0.85        63
     accuracy                           0.89       162
-   macro avg       0.86      0.90      0.87       162
-weighted avg       0.90      0.89      0.89       162
-</t>
-        </is>
-      </c>
-      <c r="L19" t="inlineStr">
-        <is>
-          <t xml:space="preserve">              precision    recall  f1-score   support
-           0       0.94      0.82      0.88       120
-           1       0.63      0.86      0.73        42
+   macro avg       0.89      0.87      0.88       162
+weighted avg       0.89      0.89      0.89       162
+</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t xml:space="preserve">              precision    recall  f1-score   support
+           0       0.75      0.77      0.76       102
+           1       0.60      0.57      0.58        60
+    accuracy                           0.70       162
+   macro avg       0.67      0.67      0.67       162
+weighted avg       0.69      0.70      0.70       162
+</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t xml:space="preserve">              precision    recall  f1-score   support
+           0       0.90      0.88      0.89       107
+           1       0.77      0.80      0.79        55
+    accuracy                           0.85       162
+   macro avg       0.83      0.84      0.84       162
+weighted avg       0.85      0.85      0.85       162
+</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t xml:space="preserve">              precision    recall  f1-score   support
+           0       0.88      0.90      0.89       102
+           1       0.82      0.78      0.80        60
+    accuracy                           0.86       162
+   macro avg       0.85      0.84      0.85       162
+weighted avg       0.86      0.86      0.86       162
+</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t xml:space="preserve">              precision    recall  f1-score   support
+           0       0.82      0.89      0.85        97
+           1       0.81      0.71      0.75        65
+    accuracy                           0.81       162
+   macro avg       0.81      0.80      0.80       162
+weighted avg       0.81      0.81      0.81       162
+</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t xml:space="preserve">              precision    recall  f1-score   support
+           0       0.87      0.88      0.88       103
+           1       0.79      0.76      0.78        59
+    accuracy                           0.84       162
+   macro avg       0.83      0.82      0.83       162
+weighted avg       0.84      0.84      0.84       162
+</t>
+        </is>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t xml:space="preserve">              precision    recall  f1-score   support
+           0       1.00      0.65      0.79       162
+           1       0.00      0.00      0.00         0
+    accuracy                           0.65       162
+   macro avg       0.50      0.32      0.39       162
+weighted avg       1.00      0.65      0.79       162
+</t>
+        </is>
+      </c>
+      <c r="L21" t="inlineStr">
+        <is>
+          <t xml:space="preserve">              precision    recall  f1-score   support
+           0       0.89      0.89      0.89       105
+           1       0.79      0.79      0.79        57
+    accuracy                           0.85       162
+   macro avg       0.84      0.84      0.84       162
+weighted avg       0.85      0.85      0.85       162
+</t>
+        </is>
+      </c>
+      <c r="M21" t="inlineStr">
+        <is>
+          <t xml:space="preserve">              precision    recall  f1-score   support
+           0       0.78      0.91      0.84        90
+           1       0.86      0.68      0.76        72
+    accuracy                           0.81       162
+   macro avg       0.82      0.80      0.80       162
+weighted avg       0.82      0.81      0.80       162
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Boruta feature selection</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t xml:space="preserve">              precision    recall  f1-score   support
+           0       0.89      0.80      0.84       116
+           1       0.60      0.74      0.66        46
+    accuracy                           0.78       162
+   macro avg       0.74      0.77      0.75       162
+weighted avg       0.80      0.78      0.79       162
+</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t xml:space="preserve">              precision    recall  f1-score   support
+           0       0.90      0.89      0.89       106
+           1       0.79      0.80      0.80        56
+    accuracy                           0.86       162
+   macro avg       0.84      0.85      0.84       162
+weighted avg       0.86      0.86      0.86       162
+</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t xml:space="preserve">              precision    recall  f1-score   support
+           0       0.91      0.88      0.90       109
+           1       0.77      0.83      0.80        53
+    accuracy                           0.86       162
+   macro avg       0.84      0.86      0.85       162
+weighted avg       0.87      0.86      0.87       162
+</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t xml:space="preserve">              precision    recall  f1-score   support
+         0.0       0.91      0.82      0.86       117
+         1.0       0.63      0.80      0.71        45
+    accuracy                           0.81       162
+   macro avg       0.77      0.81      0.79       162
+weighted avg       0.84      0.81      0.82       162
+</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t xml:space="preserve">              precision    recall  f1-score   support
+           0       0.91      0.86      0.89       111
+           1       0.74      0.82      0.78        51
+    accuracy                           0.85       162
+   macro avg       0.83      0.84      0.83       162
+weighted avg       0.86      0.85      0.85       162
+</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t xml:space="preserve">              precision    recall  f1-score   support
+           0       0.94      0.80      0.86       124
+           1       0.56      0.84      0.67        38
+    accuracy                           0.81       162
+   macro avg       0.75      0.82      0.77       162
+weighted avg       0.85      0.81      0.82       162
+</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t xml:space="preserve">              precision    recall  f1-score   support
+           0       0.94      0.79      0.86       125
+           1       0.54      0.84      0.66        37
+    accuracy                           0.80       162
+   macro avg       0.74      0.81      0.76       162
+weighted avg       0.85      0.80      0.81       162
+</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t xml:space="preserve">              precision    recall  f1-score   support
+           0       0.91      0.85      0.88       113
+           1       0.70      0.82      0.75        49
+    accuracy                           0.84       162
+   macro avg       0.81      0.83      0.82       162
+weighted avg       0.85      0.84      0.84       162
+</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t xml:space="preserve">              precision    recall  f1-score   support
+           0       0.93      0.88      0.91       111
+           1       0.77      0.86      0.81        51
+    accuracy                           0.88       162
+   macro avg       0.85      0.87      0.86       162
+weighted avg       0.88      0.88      0.88       162
+</t>
+        </is>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t xml:space="preserve">              precision    recall  f1-score   support
+           0       0.94      0.84      0.89       118
+           1       0.67      0.86      0.75        44
+    accuracy                           0.85       162
+   macro avg       0.80      0.85      0.82       162
+weighted avg       0.87      0.85      0.85       162
+</t>
+        </is>
+      </c>
+      <c r="L23" t="inlineStr">
+        <is>
+          <t xml:space="preserve">              precision    recall  f1-score   support
+           0       0.95      0.82      0.88       122
+           1       0.61      0.88      0.72        40
     accuracy                           0.83       162
-   macro avg       0.79      0.84      0.80       162
-weighted avg       0.86      0.83      0.84       162
+   macro avg       0.78      0.85      0.80       162
+weighted avg       0.87      0.83      0.84       162
+</t>
+        </is>
+      </c>
+      <c r="M23" t="inlineStr">
+        <is>
+          <t xml:space="preserve">              precision    recall  f1-score   support
+           0       0.84      0.92      0.88        96
+           1       0.86      0.74      0.80        66
+    accuracy                           0.85       162
+   macro avg       0.85      0.83      0.84       162
+weighted avg       0.85      0.85      0.84       162
 </t>
         </is>
       </c>

</xml_diff>